<commit_message>
Adição do ETL com os testes funcionando e nesse caso implementei um .env para guardar as credenciais do banco
</commit_message>
<xml_diff>
--- a/dados/dados_mercado.xlsx
+++ b/dados/dados_mercado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\limei\PycharmProjects\ETL-Excel-Oracle\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{258F5272-39D7-459F-A35C-D59AE16916BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7385FF-7F90-4DBF-9962-2A84A767CE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D038CDE-6520-4689-8050-4B6464E36719}"/>
   </bookViews>
@@ -38,19 +38,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>nomes</t>
+    <t>codigo</t>
   </si>
   <si>
-    <t>quantidades</t>
+    <t>quantidade</t>
   </si>
   <si>
-    <t>arroz</t>
+    <t>A</t>
   </si>
   <si>
-    <t>feijão</t>
+    <t>B</t>
   </si>
   <si>
-    <t>ovos</t>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>